<commit_message>
Fix write protect error in Libre
</commit_message>
<xml_diff>
--- a/Views.xlsx
+++ b/Views.xlsx
@@ -10,10 +10,10 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -103,11 +103,9 @@
   </numFmts>
   <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -191,16 +189,16 @@
   </sheetPr>
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -268,7 +266,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -276,7 +274,6 @@
         <v>22</v>
       </c>
       <c r="C2" s="0" t="n">
-        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -331,14 +328,13 @@
         <v>0.2</v>
       </c>
       <c r="U2" s="0" t="n">
-        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V2" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -346,7 +342,6 @@
         <v>22</v>
       </c>
       <c r="C3" s="0" t="n">
-        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D3" s="0" t="n">
@@ -401,14 +396,13 @@
         <v>8</v>
       </c>
       <c r="U3" s="0" t="n">
-        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V3" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -416,7 +410,6 @@
         <v>22</v>
       </c>
       <c r="C4" s="0" t="n">
-        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -471,14 +464,13 @@
         <v>2.4</v>
       </c>
       <c r="U4" s="0" t="n">
-        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V4" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
@@ -547,13 +539,12 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" password="ca3f" objects="true" scenarios="true"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data for 10 and 11
</commit_message>
<xml_diff>
--- a/Views.xlsx
+++ b/Views.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -189,13 +189,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V10"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V10" activeCellId="0" sqref="V10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U12" activeCellId="0" sqref="U12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -847,6 +847,136 @@
         <v>0.1</v>
       </c>
       <c r="U10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>9.2</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>9.4</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <v>8.3</v>
+      </c>
+      <c r="S11" s="0" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="T11" s="0" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="U11" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>14.3</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="S12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="T12" s="0" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="U12" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update analysis for table dimensions
</commit_message>
<xml_diff>
--- a/Views.xlsx
+++ b/Views.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t xml:space="preserve">I am glad it is happening</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should do research in ICU Should follow up all the patients Should see how patients are getting on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If there’s anything we can do we should do it</t>
   </si>
 </sst>
 </file>
@@ -207,10 +213,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X16"/>
+  <dimension ref="A1:X19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X17" activeCellId="0" sqref="X17"/>
+      <selection pane="topLeft" activeCell="X19" activeCellId="0" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1322,6 +1328,219 @@
       </c>
       <c r="X16" s="0" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>8.3</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>8.3</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="R17" s="0" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="S17" s="0" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="T17" s="0" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="U17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="W17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="X17" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>16.4</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="P18" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="R18" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="S18" s="0" t="n">
+        <v>16.2</v>
+      </c>
+      <c r="T18" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="U18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="W18" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>16.4</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>12.6</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P19" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q19" s="0" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="R19" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="S19" s="0" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="T19" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V19" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="W19" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="X19" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added imputed sheet to Views
</commit_message>
<xml_diff>
--- a/Views.xlsx
+++ b/Views.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Imputed" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="33">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -221,11 +222,11 @@
   </sheetPr>
   <dimension ref="A1:X22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W22" activeCellId="0" sqref="W22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1756,4 +1757,1551 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:X22"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S21" activeCellId="0" sqref="S21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>14.6</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>15.9</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>12.4</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="O2" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="S2" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="T2" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>12.9</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="O3" s="1" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="P3" s="1" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="Q3" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="S3" s="1" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="T3" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="U3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N4" s="1" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="O4" s="1" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="P4" s="1" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="Q4" s="1" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="S4" s="1" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="T4" s="1" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="U4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="N5" s="1" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="O5" s="1" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="P5" s="1" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="Q5" s="1" t="n">
+        <v>8.3</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="S5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" s="1" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="U5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>15.6</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>11.7</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="N6" s="1" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="O6" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="P6" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="Q6" s="1" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="S6" s="1" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="T6" s="1" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="U6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>13.7</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="L7" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="N7" s="1" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="O7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P7" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="Q7" s="1" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="R7" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="S7" s="1" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="T7" s="1" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="U7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>15.9</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="N8" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="O8" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="P8" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q8" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="R8" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S8" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="T8" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>13.6</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>14.9</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>14.6</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" s="1" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="P9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="1" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="R9" s="1" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="S9" s="1" t="n">
+        <v>14.6</v>
+      </c>
+      <c r="T9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="U9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>10.1</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>16.2</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="L10" s="1" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="M10" s="1" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="N10" s="1" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="O10" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P10" s="1" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="Q10" s="1" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="R10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="S10" s="1" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="T10" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="U10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>9.2</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>9.4</v>
+      </c>
+      <c r="L11" s="1" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="N11" s="1" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="O11" s="1" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="P11" s="1" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="Q11" s="1" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="R11" s="1" t="n">
+        <v>8.3</v>
+      </c>
+      <c r="S11" s="1" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="T11" s="1" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="U11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>14.3</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="L12" s="1" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="M12" s="1" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="N12" s="1" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="O12" s="1" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="P12" s="1" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="Q12" s="1" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="R12" s="1" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="S12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="T12" s="1" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="U12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>10.6</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>10.7</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>13.1</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="L13" s="1" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="N13" s="1" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="O13" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P13" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="Q13" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="R13" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S13" s="1" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="T13" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="U13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>16.4</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J14" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L14" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="M14" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N14" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="O14" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P14" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Q14" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="R14" s="1" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="S14" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="T14" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="U14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W14" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="J15" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L15" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="M15" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="N15" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="O15" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="P15" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="Q15" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="R15" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="S15" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="T15" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="U15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>12.9</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>9.2</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <v>13.8</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="J16" s="1" t="n">
+        <v>13.8</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="L16" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M16" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N16" s="1" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="O16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P16" s="1" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="Q16" s="1" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="R16" s="1" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="S16" s="1" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="T16" s="1" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="U16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>8.3</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J17" s="1" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L17" s="1" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="M17" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N17" s="1" t="n">
+        <v>8.3</v>
+      </c>
+      <c r="O17" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P17" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Q17" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="R17" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="S17" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="T17" s="1" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="U17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>16.4</v>
+      </c>
+      <c r="J18" s="1" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="L18" s="1" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="M18" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="N18" s="1" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="O18" s="1" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="P18" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q18" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="R18" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="S18" s="1" t="n">
+        <v>16.2</v>
+      </c>
+      <c r="T18" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="U18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W18" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>16.4</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>12.6</v>
+      </c>
+      <c r="J19" s="1" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="K19" s="1" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="L19" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M19" s="1" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="N19" s="1" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="O19" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P19" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q19" s="1" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="R19" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="S19" s="1" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="T19" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W19" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>8.3</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>8.3</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="P20" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="R20" s="0" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="S20" s="0" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="T20" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="U20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V20" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="W20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="X20" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>13.4</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P21" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Q21" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="R21" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="S21" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="T21" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="U21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W21" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>13.7</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="P22" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Q22" s="0" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="R22" s="0" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="S22" s="0" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="T22" s="0" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="U22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W22" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
23 and tidying graphs
</commit_message>
<xml_diff>
--- a/Views.xlsx
+++ b/Views.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="33">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -226,7 +226,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1764,13 +1764,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X22"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S21" activeCellId="0" sqref="S21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X23" activeCellId="0" sqref="X23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3292,6 +3292,74 @@
         <v>0</v>
       </c>
       <c r="W22" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>16.2</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M23" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="O23" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P23" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q23" s="0" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="R23" s="0" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="S23" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="T23" s="0" t="n">
+        <v>12.9</v>
+      </c>
+      <c r="U23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W23" s="0" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>